<commit_message>
Updated Prior beliefs and code refactoring
The code was refactored and modularised further to eliminate certain global variables that introduces bugs.
</commit_message>
<xml_diff>
--- a/EVPXIData2.xlsx
+++ b/EVPXIData2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezep\Desktop\SPARKSPECTRUM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341B3BA6-E132-4D5D-8F80-813E26D31203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tonga" sheetId="1" r:id="rId1"/>
@@ -18,18 +19,64 @@
     <sheet name="Samoa Rural" sheetId="4" r:id="rId4"/>
     <sheet name="Posterior" sheetId="6" r:id="rId5"/>
     <sheet name="Priors" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="10">
+  <si>
+    <t>Strong belief in severe outbreak</t>
+  </si>
+  <si>
+    <t>Strong belief in medium outbreak</t>
+  </si>
+  <si>
+    <t>Strong belief in low outbreak</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>Values used before</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
   </numFmts>
@@ -50,12 +97,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -70,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -86,6 +151,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -442,7 +513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -754,11 +825,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1062,11 +1133,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
@@ -1595,7 +1667,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2041,7 +2113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2218,665 +2290,1688 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G27"/>
+      <selection activeCell="B1" sqref="B1:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1">
-        <f t="shared" ref="A1:A27" si="0">1/27</f>
+        <f>1/27</f>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="B1">
+        <v>0.125</v>
+      </c>
+      <c r="C1">
+        <v>2.7E-2</v>
+      </c>
+      <c r="D1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B2">
+        <v>0.05</v>
+      </c>
+      <c r="C2">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D2">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B4">
+        <v>0.05</v>
+      </c>
+      <c r="C4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B5">
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="C5">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B6">
+        <v>0.03</v>
+      </c>
+      <c r="C6">
+        <v>0.03</v>
+      </c>
+      <c r="D6">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B7">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B8">
+        <v>0.03</v>
+      </c>
+      <c r="C8">
+        <v>0.03</v>
+      </c>
+      <c r="D8">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B9">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C9">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B10">
+        <v>0.05</v>
+      </c>
+      <c r="C10">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D10">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B11">
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="C11">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D11">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B12">
+        <v>0.03</v>
+      </c>
+      <c r="C12">
+        <v>0.03</v>
+      </c>
+      <c r="D12">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B13">
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="C13">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D13">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B14">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="C14">
+        <v>0.125</v>
+      </c>
+      <c r="D14">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B15">
+        <v>1.2000000000000002E-2</v>
+      </c>
+      <c r="C15">
+        <v>0.05</v>
+      </c>
+      <c r="D15">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B16">
+        <v>0.03</v>
+      </c>
+      <c r="C16">
+        <v>0.03</v>
+      </c>
+      <c r="D16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B17">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C17">
+        <v>0.05</v>
+      </c>
+      <c r="D17">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B18">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C18">
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="D18">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B19">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C19">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B20">
+        <v>0.03</v>
+      </c>
+      <c r="C20">
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B21">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C21">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D21">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B22">
+        <v>0.03</v>
+      </c>
+      <c r="C22">
+        <v>0.03</v>
+      </c>
+      <c r="D22">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B23">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C23">
+        <v>0.05</v>
+      </c>
+      <c r="D23">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B24">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C24">
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="D24">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B25">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C25">
+        <v>1.2000000000000002E-2</v>
+      </c>
+      <c r="D25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B26">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C26">
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="D26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <f>1/27</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="B27">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C27">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="D27">
+        <v>0.125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92019FA5-B528-4DBA-880E-B0980740CFBC}">
+  <dimension ref="B1:T34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="6.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="7.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <f>J3*K3*L3</f>
+        <v>0.125</v>
+      </c>
+      <c r="F2">
+        <f>N3*O3*P3</f>
+        <v>2.7E-2</v>
+      </c>
+      <c r="G2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>J3*K3*L4</f>
+        <v>0.05</v>
+      </c>
+      <c r="F3">
+        <f>N3*O3*P4</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>0.5</v>
+      </c>
+      <c r="K3">
+        <v>0.5</v>
+      </c>
+      <c r="L3">
+        <v>0.5</v>
+      </c>
+      <c r="N3">
+        <v>0.3</v>
+      </c>
+      <c r="O3">
+        <v>0.3</v>
+      </c>
+      <c r="P3">
+        <v>0.3</v>
+      </c>
+      <c r="R3">
+        <v>0.2</v>
+      </c>
+      <c r="S3">
+        <v>0.2</v>
+      </c>
+      <c r="T3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f>J3*K3*L5</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F4">
+        <f>N3*O3*P5</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.02</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>0.2</v>
+      </c>
+      <c r="K4">
+        <v>0.2</v>
+      </c>
+      <c r="L4">
+        <v>0.2</v>
+      </c>
+      <c r="N4">
+        <v>0.5</v>
+      </c>
+      <c r="O4">
+        <v>0.5</v>
+      </c>
+      <c r="P4">
+        <v>0.5</v>
+      </c>
+      <c r="R4">
+        <v>0.3</v>
+      </c>
+      <c r="S4">
+        <v>0.3</v>
+      </c>
+      <c r="T4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f>J3*K4*L3</f>
+        <v>0.05</v>
+      </c>
+      <c r="F5">
+        <f>N3*O4*P3</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>0.3</v>
+      </c>
+      <c r="K5">
+        <v>0.3</v>
+      </c>
+      <c r="L5">
+        <v>0.3</v>
+      </c>
+      <c r="N5">
+        <v>0.2</v>
+      </c>
+      <c r="O5">
+        <v>0.2</v>
+      </c>
+      <c r="P5">
+        <v>0.2</v>
+      </c>
+      <c r="R5">
+        <v>0.5</v>
+      </c>
+      <c r="S5">
+        <v>0.5</v>
+      </c>
+      <c r="T5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f>J3*K4*L4</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="F6">
+        <f>N3*O4*P4</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f>J3*K4*L5</f>
+        <v>0.03</v>
+      </c>
+      <c r="F7">
+        <f>N3*O4*P5</f>
+        <v>0.03</v>
+      </c>
+      <c r="G7">
+        <v>0.03</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <f>J3*K5*L3</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F8">
+        <f>N3*O5*P3</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.02</v>
+      </c>
+      <c r="K8">
         <v>0.51200000000000012</v>
       </c>
-      <c r="C1">
+      <c r="L8">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="D1">
+      <c r="M8">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="E1">
+      <c r="N8">
         <v>0.125</v>
       </c>
-      <c r="F1" s="1">
+      <c r="O8" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G1">
+      <c r="P8">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B2">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <f>J3*K5*L4</f>
+        <v>0.03</v>
+      </c>
+      <c r="F9">
+        <f>N3*O5*P4</f>
+        <v>0.03</v>
+      </c>
+      <c r="G9">
+        <v>0.03</v>
+      </c>
+      <c r="K9">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="C2">
+      <c r="L9">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="D2">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E2">
+      <c r="M9">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N9">
         <v>0.05</v>
       </c>
-      <c r="F2" s="1">
+      <c r="O9" s="1">
         <v>2.7E-2</v>
       </c>
-      <c r="G2">
+      <c r="P9">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B3">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <f>J3*K5*L5</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F10">
+        <f>N3*O5*P5</f>
+        <v>1.2E-2</v>
+      </c>
+      <c r="G10">
+        <v>0.05</v>
+      </c>
+      <c r="K10">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="C3">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D3">
+      <c r="L10">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M10">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="E3">
+      <c r="N10">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="O10" s="1">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G3">
+      <c r="P10">
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B4">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <f>J4*K3*L3</f>
+        <v>0.05</v>
+      </c>
+      <c r="F11">
+        <f>N4*O3*P3</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G11">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K11">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="C4">
+      <c r="L11">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="D4">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E4">
+      <c r="M11">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N11">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F4" s="1">
+      <c r="O11" s="1">
         <v>1.2E-2</v>
       </c>
-      <c r="G4">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B5">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C5">
+      <c r="P11">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <f>J4*K3*L4</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="F12">
+        <f>N4*O3*P4</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="K12">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L12">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="D5">
+      <c r="M12">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="E5">
-        <v>0.03</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="N12">
+        <v>0.03</v>
+      </c>
+      <c r="O12" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G5">
+      <c r="P12">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B6">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C6">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D6">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E6">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <f>J4*K3*L5</f>
+        <v>0.03</v>
+      </c>
+      <c r="F13">
+        <f>N4*O3*P5</f>
+        <v>0.03</v>
+      </c>
+      <c r="G13">
+        <v>0.03</v>
+      </c>
+      <c r="K13">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L13">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M13">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N13">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F6" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="G6">
+      <c r="O13" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="P13">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B7">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <f>J4*K4*L3</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="F14">
+        <f>N4*O4*P3</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G14">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="K14">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="C7">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D7">
+      <c r="L14">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M14">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="E7">
+      <c r="N14">
         <v>0.05</v>
       </c>
-      <c r="F7" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="G7">
+      <c r="O14" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="P14">
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B8">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C8">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D8">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E8">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <f>J4*K4*L4</f>
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="F15">
+        <f>N4*O4*P4</f>
+        <v>0.125</v>
+      </c>
+      <c r="G15">
+        <v>2.7E-2</v>
+      </c>
+      <c r="K15">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L15">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M15">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N15">
         <v>2.0000000000000004E-2</v>
       </c>
-      <c r="F8" s="1">
+      <c r="O15" s="1">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G8">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B9">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C9">
+      <c r="P15">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <f>J4*K4*L5</f>
+        <v>1.2000000000000002E-2</v>
+      </c>
+      <c r="F16">
+        <f>N4*O4*P5</f>
+        <v>0.05</v>
+      </c>
+      <c r="G16">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K16">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L16">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="D9">
+      <c r="M16">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="E9">
-        <v>0.03</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="N16">
+        <v>0.03</v>
+      </c>
+      <c r="O16" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G9">
+      <c r="P16">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B10">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <f>J4*K5*L3</f>
+        <v>0.03</v>
+      </c>
+      <c r="F17">
+        <f>N4*O5*P3</f>
+        <v>0.03</v>
+      </c>
+      <c r="G17">
+        <v>0.03</v>
+      </c>
+      <c r="K17">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="C10">
+      <c r="L17">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="D10">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E10">
+      <c r="M17">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N17">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="O17" s="1">
         <v>1.2E-2</v>
       </c>
-      <c r="G10">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B11">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C11">
+      <c r="P17">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <f>J4*K5*L4</f>
+        <v>1.2E-2</v>
+      </c>
+      <c r="F18">
+        <f>N4*O5*P4</f>
+        <v>0.05</v>
+      </c>
+      <c r="G18">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K18">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L18">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="D11">
+      <c r="M18">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="E11">
-        <v>0.03</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="N18">
+        <v>0.03</v>
+      </c>
+      <c r="O18" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G11">
+      <c r="P18">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B12">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C12">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D12">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E12">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <f>J4*K5*L5</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F19">
+        <f>N4*O5*P5</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="G19">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K19">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L19">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M19">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N19">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F12" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="G12">
+      <c r="O19" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="P19">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B13">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C13">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <f>J5*K3*L3</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F20">
+        <f>N5*O3*P3</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G20">
+        <v>0.02</v>
+      </c>
+      <c r="K20">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L20">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="D13">
+      <c r="M20">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="E13">
+      <c r="N20">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F13" s="1">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="G13">
+      <c r="O20" s="1">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="P20">
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B14">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <f>J5*K3*L4</f>
+        <v>0.03</v>
+      </c>
+      <c r="F21">
+        <f>N5*O5*P4</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="G21">
+        <v>0.03</v>
+      </c>
+      <c r="K21">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="C14">
+      <c r="L21">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="D14">
+      <c r="M21">
         <v>0.51200000000000012</v>
       </c>
-      <c r="E14">
+      <c r="N21">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F14" s="1">
+      <c r="O21" s="1">
         <v>1.2000000000000002E-2</v>
       </c>
-      <c r="G14">
+      <c r="P21">
         <v>0.125</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B15">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <f>J5*K3*L5</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F22">
+        <f>N5*O3*P5</f>
+        <v>1.2E-2</v>
+      </c>
+      <c r="G22">
+        <v>0.05</v>
+      </c>
+      <c r="K22">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="C15">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D15">
+      <c r="L22">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M22">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="E15">
+      <c r="N22">
         <v>2.7E-2</v>
       </c>
-      <c r="F15" s="1">
+      <c r="O22" s="1">
         <v>2.0000000000000004E-2</v>
       </c>
-      <c r="G15">
+      <c r="P22">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B16">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C16">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D16">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E16">
-        <v>0.03</v>
-      </c>
-      <c r="F16" s="1">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <f>J5*K4*L3</f>
+        <v>0.03</v>
+      </c>
+      <c r="F23">
+        <f>N5*O4*P3</f>
+        <v>0.03</v>
+      </c>
+      <c r="G23">
+        <v>0.03</v>
+      </c>
+      <c r="K23">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L23">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M23">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N23">
+        <v>0.03</v>
+      </c>
+      <c r="O23" s="1">
         <v>2.0000000000000004E-2</v>
       </c>
-      <c r="G16">
+      <c r="P23">
         <v>2.0000000000000004E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B17">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <f>J5*K4*L4</f>
+        <v>1.2E-2</v>
+      </c>
+      <c r="F24">
+        <f>N5*O4*P4</f>
+        <v>0.05</v>
+      </c>
+      <c r="G24">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K24">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="C17">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D17">
+      <c r="L24">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M24">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="E17">
+      <c r="N24">
         <v>1.2E-2</v>
       </c>
-      <c r="F17" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="G17">
+      <c r="O24" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="P24">
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B18">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <f>J5*K4*L5</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F25">
+        <f>N5*O4*P5</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="G25">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K25">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="C18">
+      <c r="L25">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="D18">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E18">
+      <c r="M25">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N25">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F18" s="1">
+      <c r="O25" s="1">
         <v>0.05</v>
       </c>
-      <c r="G18">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B19">
+      <c r="P25">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <f>J5*K5*L3</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F26">
+        <f>N5*O5*P3</f>
+        <v>1.2000000000000002E-2</v>
+      </c>
+      <c r="G26">
+        <v>0.05</v>
+      </c>
+      <c r="K26">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="C19">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D19">
+      <c r="L26">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M26">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="E19">
+      <c r="N26">
         <v>0.05</v>
       </c>
-      <c r="F19" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="G19">
+      <c r="O26" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="P26">
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B20">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C20">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D20">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E20">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <f>K5*J5*L4</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F27">
+        <f>N5*O5*P4</f>
         <v>2.0000000000000004E-2</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K27">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L27">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M27">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N27">
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="O27" s="1">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G20">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B21">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C21">
+      <c r="P27">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B28" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <f>J5*K5*L5</f>
+        <v>2.7E-2</v>
+      </c>
+      <c r="F28">
+        <f>N5*O5*P5</f>
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="G28">
+        <v>0.125</v>
+      </c>
+      <c r="K28">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L28">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="D21">
+      <c r="M28">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="E21">
-        <v>0.03</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="N28">
+        <v>0.03</v>
+      </c>
+      <c r="O28" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G21">
+      <c r="P28">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B22">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C22">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D22">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E22">
-        <v>0.03</v>
-      </c>
-      <c r="F22" s="1">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="K29">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L29">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M29">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N29">
+        <v>0.03</v>
+      </c>
+      <c r="O29" s="1">
         <v>2.0000000000000004E-2</v>
       </c>
-      <c r="G22">
+      <c r="P29">
         <v>2.0000000000000004E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B23">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="K30">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="C23">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="D23">
+      <c r="L30">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="M30">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="E23">
+      <c r="N30">
         <v>1.2E-2</v>
       </c>
-      <c r="F23" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="G23">
+      <c r="O30" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="P30">
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B24">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="K31">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="C24">
+      <c r="L31">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="D24">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E24">
+      <c r="M31">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N31">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F24" s="1">
+      <c r="O31" s="1">
         <v>0.05</v>
       </c>
-      <c r="G24">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B25">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="C25">
+      <c r="P31">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="K32">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="L32">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="D25">
+      <c r="M32">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="E25">
+      <c r="N32">
         <v>2.0000000000000004E-2</v>
       </c>
-      <c r="F25" s="1">
+      <c r="O32" s="1">
         <v>0.05</v>
       </c>
-      <c r="G25">
-        <v>8.0000000000000019E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B26">
+      <c r="P32">
+        <v>8.0000000000000019E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="11:16" x14ac:dyDescent="0.35">
+      <c r="K33">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="C26">
+      <c r="L33">
         <v>6.4000000000000015E-2</v>
       </c>
-      <c r="D26">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="E26">
-        <v>8.0000000000000019E-3</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="M33">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="N33">
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="O33" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G26">
+      <c r="P33">
         <v>2.0000000000000004E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="B27">
+    <row r="34" spans="11:16" x14ac:dyDescent="0.35">
+      <c r="K34">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="C27">
+      <c r="L34">
         <v>0.51200000000000012</v>
       </c>
-      <c r="D27">
+      <c r="M34">
         <v>1.0000000000000002E-3</v>
       </c>
-      <c r="E27">
+      <c r="N34">
         <v>1.2000000000000002E-2</v>
       </c>
-      <c r="F27" s="1">
+      <c r="O34" s="1">
         <v>0.125</v>
       </c>
-      <c r="G27">
+      <c r="P34">
         <v>1.2000000000000002E-2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F10 F12:F27">
+  <mergeCells count="2">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="K7:P7"/>
+  </mergeCells>
+  <conditionalFormatting sqref="O8:O17 O19:O34">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2888,7 +3983,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="O18">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2900,7 +3995,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E27">
+  <conditionalFormatting sqref="N8:N34">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2912,7 +4007,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G27">
+  <conditionalFormatting sqref="P8:P34">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>